<commit_message>
added base standards and first functions
</commit_message>
<xml_diff>
--- a/Web3 Dev Workflow - Staking contract.xlsx
+++ b/Web3 Dev Workflow - Staking contract.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USER\Downloads\ATLAS\Projects\ERC-1404 Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USER\Downloads\ATLAS\Projects\ERC-1404 Testing\security-token-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D185A4-C05A-462D-ADA6-C05C1D4C50A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB6C9BA-F68A-484C-8606-CFEC8856E3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{87969E29-7A84-4514-BDC3-69AC49AF9C42}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1253,7 @@
         <v>118</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" s="17">
         <v>3</v>
@@ -1270,7 +1270,7 @@
     <mergeCell ref="D16:D21"/>
     <mergeCell ref="C16:C21"/>
   </mergeCells>
-  <conditionalFormatting sqref="C22:C1048576 C1:C16">
+  <conditionalFormatting sqref="C1:C16 C22:C1048576">
     <cfRule type="expression" dxfId="17" priority="4">
       <formula>$C$5</formula>
     </cfRule>
@@ -1306,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0664BD-EA77-4CE6-84F7-54DC33A34CBB}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1368,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1379,7 +1379,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>